<commit_message>
[지현] buffitem fielditem 이름 맞춤
</commit_message>
<xml_diff>
--- a/Excels/ItemTable.xlsx
+++ b/Excels/ItemTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SebamoScript\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB37CD72-B1D4-4DC1-9E82-B8EE1D8EC019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2CB077-EB8B-444A-B824-56C84B6992D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="190">
   <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -646,19 +646,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>*:2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buffIconAssetPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>DoubleDice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>*:2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>buffIconAssetPath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DoubleDice</t>
   </si>
   <si>
     <t>두배 주사위 버프</t>
@@ -874,18 +870,6 @@
   </si>
   <si>
     <t>MinusDiceBuff</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MinusDice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HalfDice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Drunk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1450,7 +1434,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1459,7 +1443,7 @@
         <v>100</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1742,42 +1726,42 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1842,7 +1826,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
         <v>50</v>
@@ -1862,7 +1846,7 @@
         <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C4" t="s">
         <v>85</v>
@@ -1882,7 +1866,7 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
         <v>60</v>
@@ -1899,7 +1883,7 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
         <v>61</v>
@@ -1916,7 +1900,7 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C7" t="s">
         <v>62</v>
@@ -1933,7 +1917,7 @@
         <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C8" t="s">
         <v>69</v>
@@ -1950,7 +1934,7 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C9" t="s">
         <v>70</v>
@@ -1967,7 +1951,7 @@
         <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C10" t="s">
         <v>71</v>
@@ -1984,7 +1968,7 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
         <v>72</v>
@@ -2001,7 +1985,7 @@
         <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C12" t="s">
         <v>74</v>
@@ -2018,7 +2002,7 @@
         <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C13" t="s">
         <v>75</v>
@@ -2035,7 +2019,7 @@
         <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C14" t="s">
         <v>79</v>
@@ -2052,7 +2036,7 @@
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
         <v>80</v>
@@ -2069,7 +2053,7 @@
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C16" t="s">
         <v>81</v>
@@ -2086,7 +2070,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C17" t="s">
         <v>90</v>
@@ -2103,7 +2087,7 @@
         <v>88</v>
       </c>
       <c r="B18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
@@ -2120,7 +2104,7 @@
         <v>89</v>
       </c>
       <c r="B19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C19" t="s">
         <v>92</v>
@@ -2137,7 +2121,7 @@
         <v>98</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C20" t="s">
         <v>102</v>
@@ -2154,7 +2138,7 @@
         <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" t="s">
         <v>103</v>
@@ -2171,7 +2155,7 @@
         <v>100</v>
       </c>
       <c r="B22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C22" t="s">
         <v>104</v>
@@ -2188,7 +2172,7 @@
         <v>101</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C23" t="s">
         <v>105</v>
@@ -2253,16 +2237,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B27" t="s">
         <v>117</v>
       </c>
       <c r="C27" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" t="s">
         <v>133</v>
-      </c>
-      <c r="D27" t="s">
-        <v>134</v>
       </c>
       <c r="E27">
         <v>1000</v>
@@ -2278,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC9D8DF-8F98-4A33-894A-DEBD309AB1D5}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2323,7 +2307,7 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2331,7 +2315,7 @@
         <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -2348,7 +2332,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -2365,7 +2349,7 @@
         <v>122</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C5" t="s">
         <v>122</v>
@@ -2379,16 +2363,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E6">
         <v>-1</v>
@@ -2396,16 +2380,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>189</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E7">
         <v>-1</v>
@@ -2413,16 +2397,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E8">
         <v>-1</v>
@@ -2430,16 +2414,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E9">
         <v>-1</v>
@@ -2447,16 +2431,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" t="s">
         <v>167</v>
-      </c>
-      <c r="D10" t="s">
-        <v>168</v>
       </c>
       <c r="E10">
         <v>-1</v>
@@ -2464,16 +2448,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E11">
         <v>-1</v>
@@ -2491,7 +2475,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A8" sqref="A3:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2525,7 +2509,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
         <v>112</v>
@@ -2534,21 +2518,21 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E3">
         <v>-1</v>
@@ -2556,16 +2540,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E4">
         <v>-1</v>
@@ -2573,16 +2557,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" t="s">
         <v>173</v>
       </c>
-      <c r="B5" t="s">
-        <v>174</v>
-      </c>
       <c r="C5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E5">
         <v>-1</v>
@@ -2590,16 +2574,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" t="s">
         <v>175</v>
       </c>
-      <c r="B6" t="s">
-        <v>176</v>
-      </c>
       <c r="C6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E6">
         <v>-1</v>
@@ -2607,16 +2591,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" t="s">
         <v>177</v>
       </c>
-      <c r="B7" t="s">
-        <v>178</v>
-      </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E7">
         <v>-1</v>
@@ -2624,16 +2608,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" t="s">
         <v>179</v>
       </c>
-      <c r="B8" t="s">
-        <v>180</v>
-      </c>
       <c r="C8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D8" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E8">
         <v>-1</v>

</xml_diff>